<commit_message>
Final user list changes - 16 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032670_VerifyThatDelegateOfANonPrimaryAttendeeBankerCan_Add_View_Edit_SendNotification_Delete_TheActivity.xlsx
+++ b/TestData/TMTC0032670_VerifyThatDelegateOfANonPrimaryAttendeeBankerCan_Add_View_Edit_SendNotification_Delete_TheActivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B37F7D-127A-4DBB-8C2B-18D35EAD9670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60743A38-5720-43AE-8AF4-5A4BAF23DF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Type</t>
   </si>
@@ -133,10 +133,7 @@
     <t>Email ID</t>
   </si>
   <si>
-    <t>Gabriella Ghosn</t>
-  </si>
-  <si>
-    <t>James Craven</t>
+    <t>Thomas Bailey</t>
   </si>
 </sst>
 </file>
@@ -474,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,7 +487,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -617,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +637,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>